<commit_message>
change vestavind b from NO5 to NO3
</commit_message>
<xml_diff>
--- a/EMPIRE_extension/EMPIRE_input/Sets.xlsx
+++ b/EMPIRE_extension/EMPIRE_input/Sets.xlsx
@@ -8009,7 +8009,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>NO5</t>
+          <t>NO3</t>
         </is>
       </c>
     </row>
@@ -10824,7 +10824,7 @@
     <row r="633">
       <c r="A633" t="inlineStr">
         <is>
-          <t>NO5</t>
+          <t>NO3</t>
         </is>
       </c>
       <c r="B633" t="inlineStr">
@@ -17718,7 +17718,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>NO5</t>
+          <t>NO3</t>
         </is>
       </c>
       <c r="C398" t="inlineStr">
@@ -21708,7 +21708,7 @@
     <row r="633">
       <c r="A633" t="inlineStr">
         <is>
-          <t>NO5</t>
+          <t>NO3</t>
         </is>
       </c>
       <c r="B633" t="inlineStr">

</xml_diff>

<commit_message>
fix sets - need to incl both grounded and floating for all areas
</commit_message>
<xml_diff>
--- a/EMPIRE_extension/EMPIRE_input/Sets.xlsx
+++ b/EMPIRE_extension/EMPIRE_input/Sets.xlsx
@@ -21904,7 +21904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B773"/>
+  <dimension ref="A1:B799"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
@@ -30915,79 +30915,79 @@
     <row r="749">
       <c r="A749" t="inlineStr">
         <is>
-          <t>Moray Firth</t>
+          <t>Nordvest A</t>
         </is>
       </c>
       <c r="B749" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="750">
       <c r="A750" t="inlineStr">
         <is>
-          <t>Firth of Forth</t>
+          <t>Nordvest C</t>
         </is>
       </c>
       <c r="B750" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="751">
       <c r="A751" t="inlineStr">
         <is>
-          <t>Nordvest A</t>
+          <t>Vestavind A</t>
         </is>
       </c>
       <c r="B751" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="752">
       <c r="A752" t="inlineStr">
         <is>
-          <t>Nordvest C</t>
+          <t>Sønnavind A</t>
         </is>
       </c>
       <c r="B752" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="753">
       <c r="A753" t="inlineStr">
         <is>
-          <t>Vestavind A</t>
+          <t>Sørvest C</t>
         </is>
       </c>
       <c r="B753" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="754">
       <c r="A754" t="inlineStr">
         <is>
-          <t>Sønnavind A</t>
+          <t>Nordvest B</t>
         </is>
       </c>
       <c r="B754" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="755">
       <c r="A755" t="inlineStr">
         <is>
-          <t>Sørvest C</t>
+          <t>Vestavind F</t>
         </is>
       </c>
       <c r="B755" t="inlineStr">
@@ -30999,67 +30999,67 @@
     <row r="756">
       <c r="A756" t="inlineStr">
         <is>
-          <t>Nordvest B</t>
+          <t>Vestavind B</t>
         </is>
       </c>
       <c r="B756" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="757">
       <c r="A757" t="inlineStr">
         <is>
-          <t>Vestavind F</t>
+          <t>Vestavind C</t>
         </is>
       </c>
       <c r="B757" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="758">
       <c r="A758" t="inlineStr">
         <is>
-          <t>Vestavind B</t>
+          <t>Vestavind D</t>
         </is>
       </c>
       <c r="B758" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="759">
       <c r="A759" t="inlineStr">
         <is>
-          <t>Vestavind C</t>
+          <t>Sørvest F</t>
         </is>
       </c>
       <c r="B759" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="760">
       <c r="A760" t="inlineStr">
         <is>
-          <t>Vestavind D</t>
+          <t>Sørvest B</t>
         </is>
       </c>
       <c r="B760" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="761">
       <c r="A761" t="inlineStr">
         <is>
-          <t>Sørvest F</t>
+          <t>Nordavind B</t>
         </is>
       </c>
       <c r="B761" t="inlineStr">
@@ -31071,7 +31071,7 @@
     <row r="762">
       <c r="A762" t="inlineStr">
         <is>
-          <t>Sørvest B</t>
+          <t>Nordavind A</t>
         </is>
       </c>
       <c r="B762" t="inlineStr">
@@ -31083,79 +31083,79 @@
     <row r="763">
       <c r="A763" t="inlineStr">
         <is>
-          <t>Nordavind B</t>
+          <t>Nordavind D</t>
         </is>
       </c>
       <c r="B763" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="764">
       <c r="A764" t="inlineStr">
         <is>
-          <t>Nordavind A</t>
+          <t>Nordavind C</t>
         </is>
       </c>
       <c r="B764" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="765">
       <c r="A765" t="inlineStr">
         <is>
-          <t>Nordavind D</t>
+          <t>Vestavind E</t>
         </is>
       </c>
       <c r="B765" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="766">
       <c r="A766" t="inlineStr">
         <is>
-          <t>Nordavind C</t>
+          <t>Sørvest E</t>
         </is>
       </c>
       <c r="B766" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="767">
       <c r="A767" t="inlineStr">
         <is>
-          <t>Vestavind E</t>
+          <t>Sørvest A</t>
         </is>
       </c>
       <c r="B767" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="768">
       <c r="A768" t="inlineStr">
         <is>
-          <t>Sørvest E</t>
+          <t>Sørvest D</t>
         </is>
       </c>
       <c r="B768" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="769">
       <c r="A769" t="inlineStr">
         <is>
-          <t>Sørvest A</t>
+          <t>Moray Firth</t>
         </is>
       </c>
       <c r="B769" t="inlineStr">
@@ -31167,7 +31167,7 @@
     <row r="770">
       <c r="A770" t="inlineStr">
         <is>
-          <t>Sørvest D</t>
+          <t>Firth of Forth</t>
         </is>
       </c>
       <c r="B770" t="inlineStr">
@@ -31179,36 +31179,348 @@
     <row r="771">
       <c r="A771" t="inlineStr">
         <is>
-          <t>Sørvest E</t>
+          <t>Dogger Bank</t>
         </is>
       </c>
       <c r="B771" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="772">
       <c r="A772" t="inlineStr">
         <is>
-          <t>Sørvest A</t>
+          <t>Hornsea</t>
         </is>
       </c>
       <c r="B772" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="773">
       <c r="A773" t="inlineStr">
         <is>
+          <t>Outer Dowsing</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>Norfolk</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>East Anglia</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>Borssele</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>Hollandsee Kust</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>Helgoländer Bucht</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>Nordsøen</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>Nordvest A</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>Nordvest C</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>Vestavind A</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>Sønnavind A</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>Sørvest C</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>Nordvest B</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>Vestavind F</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>Vestavind B</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>Vestavind C</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>Vestavind D</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>Sørvest F</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>Sørvest B</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>Nordavind B</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>Nordavind A</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>Nordavind D</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>Nordavind C</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>Vestavind E</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>Sørvest E</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>Sørvest A</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
           <t>Sørvest D</t>
         </is>
       </c>
-      <c r="B773" t="inlineStr">
-        <is>
-          <t>Wind offshore grounded</t>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
clean up folder structure
</commit_message>
<xml_diff>
--- a/EMPIRE_extension/EMPIRE_input/Sets.xlsx
+++ b/EMPIRE_extension/EMPIRE_input/Sets.xlsx
@@ -28656,7 +28656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B741"/>
+  <dimension ref="A1:B733"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A664" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B694" sqref="B694"/>
@@ -36155,55 +36155,55 @@
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>Helgolander Bucht</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="624">
       <c r="A624" t="inlineStr">
         <is>
-          <t>Nordsoen</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="625">
       <c r="A625" t="inlineStr">
         <is>
-          <t>Sorlige Nordsjo I</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="626">
       <c r="A626" t="inlineStr">
         <is>
-          <t>Sorlige Nordsjo II</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="627">
       <c r="A627" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B627" t="inlineStr">
@@ -36215,7 +36215,7 @@
     <row r="628">
       <c r="A628" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>France</t>
         </is>
       </c>
       <c r="B628" t="inlineStr">
@@ -36227,7 +36227,7 @@
     <row r="629">
       <c r="A629" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Great Brit.</t>
         </is>
       </c>
       <c r="B629" t="inlineStr">
@@ -36239,7 +36239,7 @@
     <row r="630">
       <c r="A630" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="B630" t="inlineStr">
@@ -36251,7 +36251,7 @@
     <row r="631">
       <c r="A631" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="B631" t="inlineStr">
@@ -36263,7 +36263,7 @@
     <row r="632">
       <c r="A632" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="B632" t="inlineStr">
@@ -36275,7 +36275,7 @@
     <row r="633">
       <c r="A633" t="inlineStr">
         <is>
-          <t>Great Brit.</t>
+          <t>NO2</t>
         </is>
       </c>
       <c r="B633" t="inlineStr">
@@ -36287,7 +36287,7 @@
     <row r="634">
       <c r="A634" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>NO3</t>
         </is>
       </c>
       <c r="B634" t="inlineStr">
@@ -36299,7 +36299,7 @@
     <row r="635">
       <c r="A635" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>NO4</t>
         </is>
       </c>
       <c r="B635" t="inlineStr">
@@ -36311,7 +36311,7 @@
     <row r="636">
       <c r="A636" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>NO5</t>
         </is>
       </c>
       <c r="B636" t="inlineStr">
@@ -36323,103 +36323,103 @@
     <row r="637">
       <c r="A637" t="inlineStr">
         <is>
-          <t>NO2</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Nuclear</t>
         </is>
       </c>
     </row>
     <row r="638">
       <c r="A638" t="inlineStr">
         <is>
-          <t>NO3</t>
+          <t>Bosnia H</t>
         </is>
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Nuclear</t>
         </is>
       </c>
     </row>
     <row r="639">
       <c r="A639" t="inlineStr">
         <is>
-          <t>NO4</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Nuclear</t>
         </is>
       </c>
     </row>
     <row r="640">
       <c r="A640" t="inlineStr">
         <is>
-          <t>NO5</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Nuclear</t>
         </is>
       </c>
     </row>
     <row r="641">
       <c r="A641" t="inlineStr">
         <is>
-          <t>Helgolander Bucht</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Nuclear</t>
         </is>
       </c>
     </row>
     <row r="642">
       <c r="A642" t="inlineStr">
         <is>
-          <t>Nordsoen</t>
+          <t>Czech R</t>
         </is>
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Nuclear</t>
         </is>
       </c>
     </row>
     <row r="643">
       <c r="A643" t="inlineStr">
         <is>
-          <t>Sorlige Nordsjo I</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Nuclear</t>
         </is>
       </c>
     </row>
     <row r="644">
       <c r="A644" t="inlineStr">
         <is>
-          <t>Sorlige Nordsjo II</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="B644" t="inlineStr">
         <is>
-          <t>Wind offshore floating</t>
+          <t>Nuclear</t>
         </is>
       </c>
     </row>
     <row r="645">
       <c r="A645" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Estonia</t>
         </is>
       </c>
       <c r="B645" t="inlineStr">
@@ -36431,7 +36431,7 @@
     <row r="646">
       <c r="A646" t="inlineStr">
         <is>
-          <t>Bosnia H</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="B646" t="inlineStr">
@@ -36443,7 +36443,7 @@
     <row r="647">
       <c r="A647" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="B647" t="inlineStr">
@@ -36455,7 +36455,7 @@
     <row r="648">
       <c r="A648" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>France</t>
         </is>
       </c>
       <c r="B648" t="inlineStr">
@@ -36467,7 +36467,7 @@
     <row r="649">
       <c r="A649" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Great Brit.</t>
         </is>
       </c>
       <c r="B649" t="inlineStr">
@@ -36479,7 +36479,7 @@
     <row r="650">
       <c r="A650" t="inlineStr">
         <is>
-          <t>Czech R</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="B650" t="inlineStr">
@@ -36491,7 +36491,7 @@
     <row r="651">
       <c r="A651" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="B651" t="inlineStr">
@@ -36503,7 +36503,7 @@
     <row r="652">
       <c r="A652" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="B652" t="inlineStr">
@@ -36515,7 +36515,7 @@
     <row r="653">
       <c r="A653" t="inlineStr">
         <is>
-          <t>Estonia</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="B653" t="inlineStr">
@@ -36527,7 +36527,7 @@
     <row r="654">
       <c r="A654" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="B654" t="inlineStr">
@@ -36539,7 +36539,7 @@
     <row r="655">
       <c r="A655" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="B655" t="inlineStr">
@@ -36551,7 +36551,7 @@
     <row r="656">
       <c r="A656" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Luxemb.</t>
         </is>
       </c>
       <c r="B656" t="inlineStr">
@@ -36563,7 +36563,7 @@
     <row r="657">
       <c r="A657" t="inlineStr">
         <is>
-          <t>Great Brit.</t>
+          <t>Latvia</t>
         </is>
       </c>
       <c r="B657" t="inlineStr">
@@ -36575,7 +36575,7 @@
     <row r="658">
       <c r="A658" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Macedonia</t>
         </is>
       </c>
       <c r="B658" t="inlineStr">
@@ -36587,7 +36587,7 @@
     <row r="659">
       <c r="A659" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="B659" t="inlineStr">
@@ -36599,7 +36599,7 @@
     <row r="660">
       <c r="A660" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="B660" t="inlineStr">
@@ -36611,7 +36611,7 @@
     <row r="661">
       <c r="A661" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="B661" t="inlineStr">
@@ -36623,7 +36623,7 @@
     <row r="662">
       <c r="A662" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="B662" t="inlineStr">
@@ -36635,7 +36635,7 @@
     <row r="663">
       <c r="A663" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="B663" t="inlineStr">
@@ -36647,7 +36647,7 @@
     <row r="664">
       <c r="A664" t="inlineStr">
         <is>
-          <t>Luxemb.</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="B664" t="inlineStr">
@@ -36659,7 +36659,7 @@
     <row r="665">
       <c r="A665" t="inlineStr">
         <is>
-          <t>Latvia</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="B665" t="inlineStr">
@@ -36671,7 +36671,7 @@
     <row r="666">
       <c r="A666" t="inlineStr">
         <is>
-          <t>Macedonia</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="B666" t="inlineStr">
@@ -36683,7 +36683,7 @@
     <row r="667">
       <c r="A667" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>NO1</t>
         </is>
       </c>
       <c r="B667" t="inlineStr">
@@ -36695,7 +36695,7 @@
     <row r="668">
       <c r="A668" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>NO2</t>
         </is>
       </c>
       <c r="B668" t="inlineStr">
@@ -36707,7 +36707,7 @@
     <row r="669">
       <c r="A669" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>NO3</t>
         </is>
       </c>
       <c r="B669" t="inlineStr">
@@ -36719,7 +36719,7 @@
     <row r="670">
       <c r="A670" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>NO4</t>
         </is>
       </c>
       <c r="B670" t="inlineStr">
@@ -36731,7 +36731,7 @@
     <row r="671">
       <c r="A671" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>NO5</t>
         </is>
       </c>
       <c r="B671" t="inlineStr">
@@ -36743,103 +36743,103 @@
     <row r="672">
       <c r="A672" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Moray Firth</t>
         </is>
       </c>
       <c r="B672" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="673">
       <c r="A673" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Firth of Forth</t>
         </is>
       </c>
       <c r="B673" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="674">
       <c r="A674" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Dogger Bank</t>
         </is>
       </c>
       <c r="B674" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="675">
       <c r="A675" t="inlineStr">
         <is>
-          <t>NO1</t>
+          <t>Hornsea</t>
         </is>
       </c>
       <c r="B675" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="676">
       <c r="A676" t="inlineStr">
         <is>
-          <t>NO2</t>
+          <t>Outer Dowsing</t>
         </is>
       </c>
       <c r="B676" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="677">
       <c r="A677" t="inlineStr">
         <is>
-          <t>NO3</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="B677" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="678">
       <c r="A678" t="inlineStr">
         <is>
-          <t>NO4</t>
+          <t>East Anglia</t>
         </is>
       </c>
       <c r="B678" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="679">
       <c r="A679" t="inlineStr">
         <is>
-          <t>NO5</t>
+          <t>Borssele</t>
         </is>
       </c>
       <c r="B679" t="inlineStr">
         <is>
-          <t>Nuclear</t>
+          <t>Wind offshore grounded</t>
         </is>
       </c>
     </row>
     <row r="680">
       <c r="A680" t="inlineStr">
         <is>
-          <t>Moray Firth</t>
+          <t>Hollandsee Kust</t>
         </is>
       </c>
       <c r="B680" t="inlineStr">
@@ -36851,7 +36851,7 @@
     <row r="681">
       <c r="A681" t="inlineStr">
         <is>
-          <t>Firth of Forth</t>
+          <t>Helgoländer Bucht</t>
         </is>
       </c>
       <c r="B681" t="inlineStr">
@@ -36863,7 +36863,7 @@
     <row r="682">
       <c r="A682" t="inlineStr">
         <is>
-          <t>Dogger Bank</t>
+          <t>Nordsøen</t>
         </is>
       </c>
       <c r="B682" t="inlineStr">
@@ -36875,7 +36875,7 @@
     <row r="683">
       <c r="A683" t="inlineStr">
         <is>
-          <t>Hornsea</t>
+          <t>Nordvest A</t>
         </is>
       </c>
       <c r="B683" t="inlineStr">
@@ -36887,7 +36887,7 @@
     <row r="684">
       <c r="A684" t="inlineStr">
         <is>
-          <t>Outer Dowsing</t>
+          <t>Nordvest C</t>
         </is>
       </c>
       <c r="B684" t="inlineStr">
@@ -36899,7 +36899,7 @@
     <row r="685">
       <c r="A685" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Vestavind A</t>
         </is>
       </c>
       <c r="B685" t="inlineStr">
@@ -36911,7 +36911,7 @@
     <row r="686">
       <c r="A686" t="inlineStr">
         <is>
-          <t>East Anglia</t>
+          <t>Sønnavind A</t>
         </is>
       </c>
       <c r="B686" t="inlineStr">
@@ -36923,7 +36923,7 @@
     <row r="687">
       <c r="A687" t="inlineStr">
         <is>
-          <t>Borssele</t>
+          <t>Sørvest C</t>
         </is>
       </c>
       <c r="B687" t="inlineStr">
@@ -36935,7 +36935,7 @@
     <row r="688">
       <c r="A688" t="inlineStr">
         <is>
-          <t>Hollandsee Kust</t>
+          <t>Nordvest B</t>
         </is>
       </c>
       <c r="B688" t="inlineStr">
@@ -36947,7 +36947,7 @@
     <row r="689">
       <c r="A689" t="inlineStr">
         <is>
-          <t>Helgoländer Bucht</t>
+          <t>Vestavind F</t>
         </is>
       </c>
       <c r="B689" t="inlineStr">
@@ -36959,7 +36959,7 @@
     <row r="690">
       <c r="A690" t="inlineStr">
         <is>
-          <t>Nordsøen</t>
+          <t>Vestavind B</t>
         </is>
       </c>
       <c r="B690" t="inlineStr">
@@ -36971,7 +36971,7 @@
     <row r="691">
       <c r="A691" t="inlineStr">
         <is>
-          <t>Nordvest A</t>
+          <t>Vestavind C</t>
         </is>
       </c>
       <c r="B691" t="inlineStr">
@@ -36983,7 +36983,7 @@
     <row r="692">
       <c r="A692" t="inlineStr">
         <is>
-          <t>Nordvest C</t>
+          <t>Vestavind D</t>
         </is>
       </c>
       <c r="B692" t="inlineStr">
@@ -36995,7 +36995,7 @@
     <row r="693">
       <c r="A693" t="inlineStr">
         <is>
-          <t>Vestavind A</t>
+          <t>Sørvest F</t>
         </is>
       </c>
       <c r="B693" t="inlineStr">
@@ -37007,7 +37007,7 @@
     <row r="694">
       <c r="A694" t="inlineStr">
         <is>
-          <t>Sønnavind A</t>
+          <t>Sørvest B</t>
         </is>
       </c>
       <c r="B694" t="inlineStr">
@@ -37019,7 +37019,7 @@
     <row r="695">
       <c r="A695" t="inlineStr">
         <is>
-          <t>Sørvest C</t>
+          <t>Nordavind B</t>
         </is>
       </c>
       <c r="B695" t="inlineStr">
@@ -37031,7 +37031,7 @@
     <row r="696">
       <c r="A696" t="inlineStr">
         <is>
-          <t>Nordvest B</t>
+          <t>Nordavind A</t>
         </is>
       </c>
       <c r="B696" t="inlineStr">
@@ -37043,7 +37043,7 @@
     <row r="697">
       <c r="A697" t="inlineStr">
         <is>
-          <t>Vestavind F</t>
+          <t>Nordavind D</t>
         </is>
       </c>
       <c r="B697" t="inlineStr">
@@ -37055,7 +37055,7 @@
     <row r="698">
       <c r="A698" t="inlineStr">
         <is>
-          <t>Vestavind B</t>
+          <t>Nordavind C</t>
         </is>
       </c>
       <c r="B698" t="inlineStr">
@@ -37067,7 +37067,7 @@
     <row r="699">
       <c r="A699" t="inlineStr">
         <is>
-          <t>Vestavind C</t>
+          <t>Vestavind E</t>
         </is>
       </c>
       <c r="B699" t="inlineStr">
@@ -37079,7 +37079,7 @@
     <row r="700">
       <c r="A700" t="inlineStr">
         <is>
-          <t>Vestavind D</t>
+          <t>Sørvest E</t>
         </is>
       </c>
       <c r="B700" t="inlineStr">
@@ -37091,7 +37091,7 @@
     <row r="701">
       <c r="A701" t="inlineStr">
         <is>
-          <t>Sørvest F</t>
+          <t>Sørvest A</t>
         </is>
       </c>
       <c r="B701" t="inlineStr">
@@ -37103,7 +37103,7 @@
     <row r="702">
       <c r="A702" t="inlineStr">
         <is>
-          <t>Sørvest B</t>
+          <t>Sørvest D</t>
         </is>
       </c>
       <c r="B702" t="inlineStr">
@@ -37115,103 +37115,103 @@
     <row r="703">
       <c r="A703" t="inlineStr">
         <is>
-          <t>Nordavind B</t>
+          <t>Moray Firth</t>
         </is>
       </c>
       <c r="B703" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="704">
       <c r="A704" t="inlineStr">
         <is>
-          <t>Nordavind A</t>
+          <t>Firth of Forth</t>
         </is>
       </c>
       <c r="B704" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="705">
       <c r="A705" t="inlineStr">
         <is>
-          <t>Nordavind D</t>
+          <t>Dogger Bank</t>
         </is>
       </c>
       <c r="B705" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="706">
       <c r="A706" t="inlineStr">
         <is>
-          <t>Nordavind C</t>
+          <t>Hornsea</t>
         </is>
       </c>
       <c r="B706" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="707">
       <c r="A707" t="inlineStr">
         <is>
-          <t>Vestavind E</t>
+          <t>Outer Dowsing</t>
         </is>
       </c>
       <c r="B707" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="708">
       <c r="A708" t="inlineStr">
         <is>
-          <t>Sørvest E</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="B708" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="709">
       <c r="A709" t="inlineStr">
         <is>
-          <t>Sørvest A</t>
+          <t>East Anglia</t>
         </is>
       </c>
       <c r="B709" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="710">
       <c r="A710" t="inlineStr">
         <is>
-          <t>Sørvest D</t>
+          <t>Borssele</t>
         </is>
       </c>
       <c r="B710" t="inlineStr">
         <is>
-          <t>Wind offshore grounded</t>
+          <t>Wind offshore floating</t>
         </is>
       </c>
     </row>
     <row r="711">
       <c r="A711" t="inlineStr">
         <is>
-          <t>Moray Firth</t>
+          <t>Hollandsee Kust</t>
         </is>
       </c>
       <c r="B711" t="inlineStr">
@@ -37223,7 +37223,7 @@
     <row r="712">
       <c r="A712" t="inlineStr">
         <is>
-          <t>Firth of Forth</t>
+          <t>Helgoländer Bucht</t>
         </is>
       </c>
       <c r="B712" t="inlineStr">
@@ -37235,7 +37235,7 @@
     <row r="713">
       <c r="A713" t="inlineStr">
         <is>
-          <t>Dogger Bank</t>
+          <t>Nordsøen</t>
         </is>
       </c>
       <c r="B713" t="inlineStr">
@@ -37247,7 +37247,7 @@
     <row r="714">
       <c r="A714" t="inlineStr">
         <is>
-          <t>Hornsea</t>
+          <t>Nordvest A</t>
         </is>
       </c>
       <c r="B714" t="inlineStr">
@@ -37259,7 +37259,7 @@
     <row r="715">
       <c r="A715" t="inlineStr">
         <is>
-          <t>Outer Dowsing</t>
+          <t>Nordvest C</t>
         </is>
       </c>
       <c r="B715" t="inlineStr">
@@ -37271,7 +37271,7 @@
     <row r="716">
       <c r="A716" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Vestavind A</t>
         </is>
       </c>
       <c r="B716" t="inlineStr">
@@ -37283,7 +37283,7 @@
     <row r="717">
       <c r="A717" t="inlineStr">
         <is>
-          <t>East Anglia</t>
+          <t>Sønnavind A</t>
         </is>
       </c>
       <c r="B717" t="inlineStr">
@@ -37295,7 +37295,7 @@
     <row r="718">
       <c r="A718" t="inlineStr">
         <is>
-          <t>Borssele</t>
+          <t>Sørvest C</t>
         </is>
       </c>
       <c r="B718" t="inlineStr">
@@ -37307,7 +37307,7 @@
     <row r="719">
       <c r="A719" t="inlineStr">
         <is>
-          <t>Hollandsee Kust</t>
+          <t>Nordvest B</t>
         </is>
       </c>
       <c r="B719" t="inlineStr">
@@ -37319,7 +37319,7 @@
     <row r="720">
       <c r="A720" t="inlineStr">
         <is>
-          <t>Helgoländer Bucht</t>
+          <t>Vestavind F</t>
         </is>
       </c>
       <c r="B720" t="inlineStr">
@@ -37331,7 +37331,7 @@
     <row r="721">
       <c r="A721" t="inlineStr">
         <is>
-          <t>Nordsøen</t>
+          <t>Vestavind B</t>
         </is>
       </c>
       <c r="B721" t="inlineStr">
@@ -37343,7 +37343,7 @@
     <row r="722">
       <c r="A722" t="inlineStr">
         <is>
-          <t>Nordvest A</t>
+          <t>Vestavind C</t>
         </is>
       </c>
       <c r="B722" t="inlineStr">
@@ -37355,7 +37355,7 @@
     <row r="723">
       <c r="A723" t="inlineStr">
         <is>
-          <t>Nordvest C</t>
+          <t>Vestavind D</t>
         </is>
       </c>
       <c r="B723" t="inlineStr">
@@ -37367,7 +37367,7 @@
     <row r="724">
       <c r="A724" t="inlineStr">
         <is>
-          <t>Vestavind A</t>
+          <t>Sørvest F</t>
         </is>
       </c>
       <c r="B724" t="inlineStr">
@@ -37379,7 +37379,7 @@
     <row r="725">
       <c r="A725" t="inlineStr">
         <is>
-          <t>Sønnavind A</t>
+          <t>Sørvest B</t>
         </is>
       </c>
       <c r="B725" t="inlineStr">
@@ -37391,7 +37391,7 @@
     <row r="726">
       <c r="A726" t="inlineStr">
         <is>
-          <t>Sørvest C</t>
+          <t>Nordavind B</t>
         </is>
       </c>
       <c r="B726" t="inlineStr">
@@ -37403,7 +37403,7 @@
     <row r="727">
       <c r="A727" t="inlineStr">
         <is>
-          <t>Nordvest B</t>
+          <t>Nordavind A</t>
         </is>
       </c>
       <c r="B727" t="inlineStr">
@@ -37415,7 +37415,7 @@
     <row r="728">
       <c r="A728" t="inlineStr">
         <is>
-          <t>Vestavind F</t>
+          <t>Nordavind D</t>
         </is>
       </c>
       <c r="B728" t="inlineStr">
@@ -37427,7 +37427,7 @@
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>Vestavind B</t>
+          <t>Nordavind C</t>
         </is>
       </c>
       <c r="B729" t="inlineStr">
@@ -37439,7 +37439,7 @@
     <row r="730">
       <c r="A730" t="inlineStr">
         <is>
-          <t>Vestavind C</t>
+          <t>Vestavind E</t>
         </is>
       </c>
       <c r="B730" t="inlineStr">
@@ -37451,7 +37451,7 @@
     <row r="731">
       <c r="A731" t="inlineStr">
         <is>
-          <t>Vestavind D</t>
+          <t>Sørvest E</t>
         </is>
       </c>
       <c r="B731" t="inlineStr">
@@ -37463,7 +37463,7 @@
     <row r="732">
       <c r="A732" t="inlineStr">
         <is>
-          <t>Sørvest F</t>
+          <t>Sørvest A</t>
         </is>
       </c>
       <c r="B732" t="inlineStr">
@@ -37475,106 +37475,10 @@
     <row r="733">
       <c r="A733" t="inlineStr">
         <is>
-          <t>Sørvest B</t>
+          <t>Sørvest D</t>
         </is>
       </c>
       <c r="B733" t="inlineStr">
-        <is>
-          <t>Wind offshore floating</t>
-        </is>
-      </c>
-    </row>
-    <row r="734">
-      <c r="A734" t="inlineStr">
-        <is>
-          <t>Nordavind B</t>
-        </is>
-      </c>
-      <c r="B734" t="inlineStr">
-        <is>
-          <t>Wind offshore floating</t>
-        </is>
-      </c>
-    </row>
-    <row r="735">
-      <c r="A735" t="inlineStr">
-        <is>
-          <t>Nordavind A</t>
-        </is>
-      </c>
-      <c r="B735" t="inlineStr">
-        <is>
-          <t>Wind offshore floating</t>
-        </is>
-      </c>
-    </row>
-    <row r="736">
-      <c r="A736" t="inlineStr">
-        <is>
-          <t>Nordavind D</t>
-        </is>
-      </c>
-      <c r="B736" t="inlineStr">
-        <is>
-          <t>Wind offshore floating</t>
-        </is>
-      </c>
-    </row>
-    <row r="737">
-      <c r="A737" t="inlineStr">
-        <is>
-          <t>Nordavind C</t>
-        </is>
-      </c>
-      <c r="B737" t="inlineStr">
-        <is>
-          <t>Wind offshore floating</t>
-        </is>
-      </c>
-    </row>
-    <row r="738">
-      <c r="A738" t="inlineStr">
-        <is>
-          <t>Vestavind E</t>
-        </is>
-      </c>
-      <c r="B738" t="inlineStr">
-        <is>
-          <t>Wind offshore floating</t>
-        </is>
-      </c>
-    </row>
-    <row r="739">
-      <c r="A739" t="inlineStr">
-        <is>
-          <t>Sørvest E</t>
-        </is>
-      </c>
-      <c r="B739" t="inlineStr">
-        <is>
-          <t>Wind offshore floating</t>
-        </is>
-      </c>
-    </row>
-    <row r="740">
-      <c r="A740" t="inlineStr">
-        <is>
-          <t>Sørvest A</t>
-        </is>
-      </c>
-      <c r="B740" t="inlineStr">
-        <is>
-          <t>Wind offshore floating</t>
-        </is>
-      </c>
-    </row>
-    <row r="741">
-      <c r="A741" t="inlineStr">
-        <is>
-          <t>Sørvest D</t>
-        </is>
-      </c>
-      <c r="B741" t="inlineStr">
         <is>
           <t>Wind offshore floating</t>
         </is>

</xml_diff>